<commit_message>
Update of all values to match PDF edition 10 (commit 1)
</commit_message>
<xml_diff>
--- a/data/aircraft_operating_costs.xlsx
+++ b/data/aircraft_operating_costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1520082-4DB0-4B91-A79C-1628A8EC359F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A069D25-09D4-456D-903D-12FDB59B59BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aircraft_operating_costs" sheetId="1" r:id="rId1"/>
@@ -85,19 +85,19 @@
     <t>Aircraft.type</t>
   </si>
   <si>
-    <t>per.aircraft.per.year..USD.million.</t>
-  </si>
-  <si>
-    <t>per.flight.hour</t>
-  </si>
-  <si>
-    <t>per.flight.cycle</t>
-  </si>
-  <si>
-    <t>per.available.seat.Km..US.cents.</t>
-  </si>
-  <si>
-    <t>per.available.ton.km..US.cents..</t>
+    <t>per_aircraft</t>
+  </si>
+  <si>
+    <t>per_flt_hr</t>
+  </si>
+  <si>
+    <t>per_ton_km</t>
+  </si>
+  <si>
+    <t>per_seats</t>
+  </si>
+  <si>
+    <t>per_flt_cycle</t>
   </si>
 </sst>
 </file>
@@ -642,9 +642,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -682,7 +682,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -788,7 +788,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -930,7 +930,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -941,7 +941,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,13 +965,13 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>